<commit_message>
adds updated data files
</commit_message>
<xml_diff>
--- a/data-raw/lower_feather_release.xlsx
+++ b/data-raw/lower_feather_release.xlsx
@@ -2241,7 +2241,7 @@
       </c>
       <c r="C32" s="0" t="inlineStr">
         <is>
-          <t>Not applicable (n/a)</t>
+          <t>Chinook salmon</t>
         </is>
       </c>
       <c r="D32" s="0" t="inlineStr">
@@ -2298,7 +2298,7 @@
       </c>
       <c r="C33" s="0" t="inlineStr">
         <is>
-          <t>Not applicable (n/a)</t>
+          <t>Chinook salmon</t>
         </is>
       </c>
       <c r="D33" s="0" t="inlineStr">

</xml_diff>